<commit_message>
Update up to 15th may
</commit_message>
<xml_diff>
--- a/Attandance/Attendance.xlsx
+++ b/Attandance/Attendance.xlsx
@@ -5,18 +5,19 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/pothuriraju/Documents/Attandance Format/2021/Wt/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/pothuriraju/Documents/Attandance Format/2021/300Link/Attandance/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B7437585-7556-464C-87E9-08DA64B926A6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{671A8DD9-6F10-784C-9457-9472CEB50AD0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6560" yWindow="1040" windowWidth="23340" windowHeight="19360" activeTab="3" xr2:uid="{9D5B50D6-B844-0C48-B9BD-4B1296589F28}"/>
+    <workbookView xWindow="320" yWindow="500" windowWidth="21900" windowHeight="19360" activeTab="4" xr2:uid="{9D5B50D6-B844-0C48-B9BD-4B1296589F28}"/>
   </bookViews>
   <sheets>
     <sheet name="Main" sheetId="1" r:id="rId1"/>
     <sheet name="22april to 24arpil" sheetId="3" r:id="rId2"/>
     <sheet name="26th april to 1st may" sheetId="2" r:id="rId3"/>
     <sheet name="3rd May to 8th May" sheetId="4" r:id="rId4"/>
+    <sheet name="10th May to 15th May" sheetId="5" r:id="rId5"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Main!$A$1:$F$32</definedName>
@@ -39,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="295" uniqueCount="136">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="360" uniqueCount="172">
   <si>
     <t>Day</t>
   </si>
@@ -447,6 +448,114 @@
   </si>
   <si>
     <t>Time diffence</t>
+  </si>
+  <si>
+    <t>10/05/21_mon_1_9.00-9.50_WT_PRSS</t>
+  </si>
+  <si>
+    <t>10/05/21_mon_2_10.00-10.50_OOSE_SVR/TR</t>
+  </si>
+  <si>
+    <t>10/05/21_mon_3_11.00-11.50_CNS_BVDS/MKSV</t>
+  </si>
+  <si>
+    <t>10/05/21_mon_4_12.00-12.50_SRP_NRD</t>
+  </si>
+  <si>
+    <t>10/05/21_mon_5,6_2.00-3.50_QA_BRB</t>
+  </si>
+  <si>
+    <t>10/05/21_mon_7_4.00-4.50_SS_Neelima</t>
+  </si>
+  <si>
+    <t>11/05/21_tue_1_9.00-9.50_DWDBA_MVS/PNT</t>
+  </si>
+  <si>
+    <t>11/05/21_tue_2_10.00-10.50_OR_CHGR/KSB</t>
+  </si>
+  <si>
+    <t>11/05/21_tue_3_11.00-11.50_WT_PRSS</t>
+  </si>
+  <si>
+    <t>11/05/21_tue_4_12.00-12.50_OOSE_SVR/TR</t>
+  </si>
+  <si>
+    <t>11/05/21_tue_5,6_2.00-3.50_VA_MdRiaz</t>
+  </si>
+  <si>
+    <t>11/05/21_tue_7_4.00-4.50_SRP_NRD</t>
+  </si>
+  <si>
+    <t>12/05/21_wed_1_9.00-11.50_CC-II_PSR/Chandu</t>
+  </si>
+  <si>
+    <t>12/05/21_wed_4_12.00-12.50_CNS_BVDS/MKSV</t>
+  </si>
+  <si>
+    <t>12/05/21_wed_5,6,7_2.00-4.50_OOSE-LAB_SVR/TR</t>
+  </si>
+  <si>
+    <t>13/05/21_thu_1_9.00-9.50_OOSE_SVR/TR</t>
+  </si>
+  <si>
+    <t>13/05/21_thu_2_10.00-10.50_DWDBA_MVS/PNT</t>
+  </si>
+  <si>
+    <t>13/05/21_thu_3_11.00-11.50_CNS_BVDS/MKSV</t>
+  </si>
+  <si>
+    <t>13/05/21_thu_4_12.00-12.50_SRP_NRD</t>
+  </si>
+  <si>
+    <t>13/05/21_thu_5_2.00-2.50_WT_PRSS</t>
+  </si>
+  <si>
+    <t>13/05/21_thu_6_3.00-3.50_OR_CHGR/KSB</t>
+  </si>
+  <si>
+    <t>14/05/21_fri_1_9.00-9.50_DWDBA_MVS/PNT</t>
+  </si>
+  <si>
+    <t>14/05/21_fri_2_10.00-10.50_OR_CHGR/KSB</t>
+  </si>
+  <si>
+    <t>14/05/21_fri_3_11.00-11.50_OOSE_SVR/TR</t>
+  </si>
+  <si>
+    <t>14/05/21_fri_4_12.00-12.50_WT_PRSS</t>
+  </si>
+  <si>
+    <t>14/05/21_fri_5,6,7_2.00-4.50_WT LAB_PRSS</t>
+  </si>
+  <si>
+    <t>15/05/21_sat_1_9.00-9.50_CNS_BVDS/MKSV</t>
+  </si>
+  <si>
+    <t>15/05/21_sat_2_10.00-10.50_SRP_NRD</t>
+  </si>
+  <si>
+    <t>15/05/21_sat_3_11.00-11.50_DWDBA_MVS/PNT</t>
+  </si>
+  <si>
+    <t>15/05/21_sat_4_12.00-12.50_OR_CHGR/KSB</t>
+  </si>
+  <si>
+    <t>15/05/21_sat_5,6_2.00-3.50_IPR&amp;P_SR</t>
+  </si>
+  <si>
+    <t>72 studnets</t>
+  </si>
+  <si>
+    <t>NO -Lab</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Same time </t>
+  </si>
+  <si>
+    <t>holiday</t>
+  </si>
+  <si>
+    <t>NO-Class</t>
   </si>
 </sst>
 </file>
@@ -825,8 +934,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8039E4DD-5CE4-E44B-9CBA-DC1D8D4E8278}">
   <dimension ref="A1:F32"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:F32"/>
+    <sheetView zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
+      <selection activeCell="G18" sqref="G18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -853,7 +962,7 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" s="1">
-        <v>44319</v>
+        <v>44326</v>
       </c>
       <c r="B2" t="s">
         <v>5</v>
@@ -873,7 +982,7 @@
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" s="1">
-        <v>44319</v>
+        <v>44326</v>
       </c>
       <c r="B3" t="s">
         <v>5</v>
@@ -893,7 +1002,7 @@
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" s="1">
-        <v>44319</v>
+        <v>44326</v>
       </c>
       <c r="B4" t="s">
         <v>5</v>
@@ -913,7 +1022,7 @@
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" s="1">
-        <v>44319</v>
+        <v>44326</v>
       </c>
       <c r="B5" t="s">
         <v>5</v>
@@ -933,7 +1042,7 @@
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" s="1">
-        <v>44319</v>
+        <v>44326</v>
       </c>
       <c r="B6" t="s">
         <v>5</v>
@@ -953,7 +1062,7 @@
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7" s="1">
-        <v>44319</v>
+        <v>44326</v>
       </c>
       <c r="B7" t="s">
         <v>5</v>
@@ -973,7 +1082,7 @@
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8" s="1">
-        <v>44320</v>
+        <v>44327</v>
       </c>
       <c r="B8" t="s">
         <v>6</v>
@@ -993,7 +1102,7 @@
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A9" s="1">
-        <v>44320</v>
+        <v>44327</v>
       </c>
       <c r="B9" t="s">
         <v>6</v>
@@ -1013,7 +1122,7 @@
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A10" s="1">
-        <v>44320</v>
+        <v>44327</v>
       </c>
       <c r="B10" t="s">
         <v>6</v>
@@ -1033,7 +1142,7 @@
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A11" s="1">
-        <v>44320</v>
+        <v>44327</v>
       </c>
       <c r="B11" t="s">
         <v>6</v>
@@ -1053,7 +1162,7 @@
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A12" s="1">
-        <v>44320</v>
+        <v>44327</v>
       </c>
       <c r="B12" t="s">
         <v>6</v>
@@ -1073,7 +1182,7 @@
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A13" s="1">
-        <v>44320</v>
+        <v>44327</v>
       </c>
       <c r="B13" t="s">
         <v>6</v>
@@ -1093,7 +1202,7 @@
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A14" s="4">
-        <v>44321</v>
+        <v>44328</v>
       </c>
       <c r="B14" t="s">
         <v>7</v>
@@ -1113,7 +1222,7 @@
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A15" s="4">
-        <v>44321</v>
+        <v>44328</v>
       </c>
       <c r="B15" t="s">
         <v>7</v>
@@ -1133,7 +1242,7 @@
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A16" s="4">
-        <v>44321</v>
+        <v>44328</v>
       </c>
       <c r="B16" t="s">
         <v>7</v>
@@ -1153,7 +1262,7 @@
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A17" s="4">
-        <v>44321</v>
+        <v>44329</v>
       </c>
       <c r="B17" t="s">
         <v>8</v>
@@ -1172,8 +1281,8 @@
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A18" s="1">
-        <v>44322</v>
+      <c r="A18" s="4">
+        <v>44329</v>
       </c>
       <c r="B18" t="s">
         <v>8</v>
@@ -1192,8 +1301,8 @@
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A19" s="1">
-        <v>44322</v>
+      <c r="A19" s="4">
+        <v>44329</v>
       </c>
       <c r="B19" t="s">
         <v>8</v>
@@ -1212,8 +1321,8 @@
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A20" s="1">
-        <v>44322</v>
+      <c r="A20" s="4">
+        <v>44329</v>
       </c>
       <c r="B20" t="s">
         <v>8</v>
@@ -1232,8 +1341,8 @@
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A21" s="1">
-        <v>44322</v>
+      <c r="A21" s="4">
+        <v>44329</v>
       </c>
       <c r="B21" t="s">
         <v>8</v>
@@ -1252,8 +1361,8 @@
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A22" s="1">
-        <v>44322</v>
+      <c r="A22" s="4">
+        <v>44329</v>
       </c>
       <c r="B22" t="s">
         <v>8</v>
@@ -1273,7 +1382,7 @@
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A23" s="1">
-        <v>44323</v>
+        <v>44330</v>
       </c>
       <c r="B23" t="s">
         <v>9</v>
@@ -1293,7 +1402,7 @@
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A24" s="1">
-        <v>44323</v>
+        <v>44330</v>
       </c>
       <c r="B24" t="s">
         <v>9</v>
@@ -1313,7 +1422,7 @@
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A25" s="1">
-        <v>44323</v>
+        <v>44330</v>
       </c>
       <c r="B25" t="s">
         <v>9</v>
@@ -1333,7 +1442,7 @@
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A26" s="1">
-        <v>44323</v>
+        <v>44330</v>
       </c>
       <c r="B26" t="s">
         <v>9</v>
@@ -1353,7 +1462,7 @@
     </row>
     <row r="27" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A27" s="1">
-        <v>44323</v>
+        <v>44330</v>
       </c>
       <c r="B27" t="s">
         <v>9</v>
@@ -1373,7 +1482,7 @@
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A28" s="1">
-        <v>44324</v>
+        <v>44331</v>
       </c>
       <c r="B28" t="s">
         <v>10</v>
@@ -1393,7 +1502,7 @@
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A29" s="1">
-        <v>44324</v>
+        <v>44331</v>
       </c>
       <c r="B29" t="s">
         <v>10</v>
@@ -1413,7 +1522,7 @@
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A30" s="1">
-        <v>44324</v>
+        <v>44331</v>
       </c>
       <c r="B30" t="s">
         <v>10</v>
@@ -1433,7 +1542,7 @@
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A31" s="1">
-        <v>44324</v>
+        <v>44331</v>
       </c>
       <c r="B31" t="s">
         <v>10</v>
@@ -1453,7 +1562,7 @@
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A32" s="1">
-        <v>44324</v>
+        <v>44331</v>
       </c>
       <c r="B32" t="s">
         <v>10</v>
@@ -2044,8 +2153,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E25234DE-9FB1-5D40-B8A1-DF64F10F9F13}">
   <dimension ref="A2:D32"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="D33" sqref="D33"/>
+    <sheetView zoomScale="119" zoomScaleNormal="119" workbookViewId="0">
+      <selection activeCell="H30" sqref="H30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2421,4 +2530,375 @@
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{214CB285-D67A-E44B-924A-EE7C0E27AD7D}">
+  <dimension ref="B6:E36"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F38" sqref="F38"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="3" max="3" width="44.83203125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="6" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B6">
+        <v>1</v>
+      </c>
+      <c r="C6" t="s">
+        <v>136</v>
+      </c>
+      <c r="D6" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="7" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B7">
+        <v>2</v>
+      </c>
+      <c r="C7" t="s">
+        <v>137</v>
+      </c>
+      <c r="D7" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="8" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B8">
+        <v>3</v>
+      </c>
+      <c r="C8" t="s">
+        <v>138</v>
+      </c>
+      <c r="D8" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="9" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B9">
+        <v>4</v>
+      </c>
+      <c r="C9" t="s">
+        <v>139</v>
+      </c>
+      <c r="D9" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="10" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B10">
+        <v>5</v>
+      </c>
+      <c r="C10" t="s">
+        <v>140</v>
+      </c>
+      <c r="D10" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="11" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B11">
+        <v>6</v>
+      </c>
+      <c r="C11" t="s">
+        <v>141</v>
+      </c>
+      <c r="D11" t="s">
+        <v>52</v>
+      </c>
+      <c r="E11" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="12" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B12">
+        <v>7</v>
+      </c>
+      <c r="C12" t="s">
+        <v>142</v>
+      </c>
+      <c r="D12" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="13" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B13">
+        <v>8</v>
+      </c>
+      <c r="C13" t="s">
+        <v>143</v>
+      </c>
+      <c r="D13" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="14" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B14">
+        <v>9</v>
+      </c>
+      <c r="C14" t="s">
+        <v>144</v>
+      </c>
+      <c r="D14" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="15" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B15">
+        <v>10</v>
+      </c>
+      <c r="C15" t="s">
+        <v>145</v>
+      </c>
+      <c r="D15" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="16" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B16">
+        <v>11</v>
+      </c>
+      <c r="C16" t="s">
+        <v>146</v>
+      </c>
+      <c r="D16" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="17" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B17">
+        <v>12</v>
+      </c>
+      <c r="C17" t="s">
+        <v>147</v>
+      </c>
+      <c r="D17" t="s">
+        <v>52</v>
+      </c>
+      <c r="E17">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="18" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B18">
+        <v>13</v>
+      </c>
+      <c r="C18" t="s">
+        <v>148</v>
+      </c>
+      <c r="D18" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="19" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B19">
+        <v>14</v>
+      </c>
+      <c r="C19" t="s">
+        <v>149</v>
+      </c>
+      <c r="D19" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="20" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B20">
+        <v>15</v>
+      </c>
+      <c r="C20" t="s">
+        <v>150</v>
+      </c>
+      <c r="D20" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="21" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B21">
+        <v>16</v>
+      </c>
+      <c r="C21" t="s">
+        <v>151</v>
+      </c>
+      <c r="D21" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="22" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B22">
+        <v>17</v>
+      </c>
+      <c r="C22" t="s">
+        <v>152</v>
+      </c>
+      <c r="D22" t="s">
+        <v>52</v>
+      </c>
+      <c r="E22" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="23" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B23">
+        <v>18</v>
+      </c>
+      <c r="C23" t="s">
+        <v>153</v>
+      </c>
+      <c r="D23" t="s">
+        <v>52</v>
+      </c>
+      <c r="E23" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="24" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B24">
+        <v>19</v>
+      </c>
+      <c r="C24" t="s">
+        <v>154</v>
+      </c>
+      <c r="D24" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="25" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B25">
+        <v>20</v>
+      </c>
+      <c r="C25" t="s">
+        <v>155</v>
+      </c>
+      <c r="D25" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="26" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B26">
+        <v>21</v>
+      </c>
+      <c r="C26" t="s">
+        <v>156</v>
+      </c>
+      <c r="D26" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="27" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B27">
+        <v>22</v>
+      </c>
+      <c r="C27" t="s">
+        <v>157</v>
+      </c>
+      <c r="D27" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="28" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B28">
+        <v>23</v>
+      </c>
+      <c r="C28" t="s">
+        <v>158</v>
+      </c>
+      <c r="D28" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="29" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B29">
+        <v>24</v>
+      </c>
+      <c r="C29" t="s">
+        <v>159</v>
+      </c>
+      <c r="D29" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="30" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B30">
+        <v>25</v>
+      </c>
+      <c r="C30" t="s">
+        <v>160</v>
+      </c>
+      <c r="D30" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="31" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B31">
+        <v>26</v>
+      </c>
+      <c r="C31" t="s">
+        <v>161</v>
+      </c>
+      <c r="D31" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="32" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B32">
+        <v>27</v>
+      </c>
+      <c r="C32" t="s">
+        <v>162</v>
+      </c>
+      <c r="D32" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="33" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B33">
+        <v>28</v>
+      </c>
+      <c r="C33" t="s">
+        <v>163</v>
+      </c>
+      <c r="D33" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="34" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B34">
+        <v>29</v>
+      </c>
+      <c r="C34" t="s">
+        <v>164</v>
+      </c>
+      <c r="D34" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="35" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B35">
+        <v>30</v>
+      </c>
+      <c r="C35" t="s">
+        <v>165</v>
+      </c>
+      <c r="D35" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="36" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B36">
+        <v>31</v>
+      </c>
+      <c r="C36" t="s">
+        <v>166</v>
+      </c>
+      <c r="D36" t="s">
+        <v>171</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Updated upto 5th June
</commit_message>
<xml_diff>
--- a/Attandance/Attendance.xlsx
+++ b/Attandance/Attendance.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/pothuriraju/Documents/Attandance Format/2021/300Link/Attandance/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C94983D0-54F5-F04E-A5C1-84A54EC44BE6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA407CB9-1D07-444A-978F-CD1135092399}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="12280" yWindow="500" windowWidth="27220" windowHeight="19360" activeTab="6" xr2:uid="{9D5B50D6-B844-0C48-B9BD-4B1296589F28}"/>
+    <workbookView xWindow="18980" yWindow="580" windowWidth="27220" windowHeight="19360" activeTab="6" xr2:uid="{9D5B50D6-B844-0C48-B9BD-4B1296589F28}"/>
   </bookViews>
   <sheets>
     <sheet name="Main" sheetId="1" r:id="rId1"/>
@@ -18,8 +18,9 @@
     <sheet name="26th april to 1st may" sheetId="2" r:id="rId3"/>
     <sheet name="3rd May to 8th May" sheetId="4" r:id="rId4"/>
     <sheet name="10th May to 15th May" sheetId="5" r:id="rId5"/>
-    <sheet name="17th May" sheetId="6" r:id="rId6"/>
-    <sheet name="24-29" sheetId="7" r:id="rId7"/>
+    <sheet name="17th May-22 May" sheetId="6" r:id="rId6"/>
+    <sheet name="31May-5thJun" sheetId="8" r:id="rId7"/>
+    <sheet name="24th May -29th May" sheetId="7" r:id="rId8"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Main!$A$1:$F$32</definedName>
@@ -42,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="489" uniqueCount="240">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="553" uniqueCount="272">
   <si>
     <t>Day</t>
   </si>
@@ -762,6 +763,102 @@
   </si>
   <si>
     <t>Not Conducted or merged in Above class</t>
+  </si>
+  <si>
+    <t>31/05/21_mon_1_9.00-9.50_WT_PRSS</t>
+  </si>
+  <si>
+    <t>31/05/21_mon_2_10.00-10.50_OOSE_SVR/TR</t>
+  </si>
+  <si>
+    <t>31/05/21_mon_3_11.00-11.50_CNS_BVDS/MKSV</t>
+  </si>
+  <si>
+    <t>31/05/21_mon_4_12.00-12.50_SRP_NRD</t>
+  </si>
+  <si>
+    <t>31/05/21_mon_5,6_2.00-3.50_QA_BRB</t>
+  </si>
+  <si>
+    <t>31/05/21_mon_7_4.00-4.50_SS_Neelima</t>
+  </si>
+  <si>
+    <t>01/06/21_tue_1_9.00-9.50_DWDBA_MVS/PNT</t>
+  </si>
+  <si>
+    <t>01/06/21_tue_2_10.00-10.50_OR_CHGR/KSB</t>
+  </si>
+  <si>
+    <t>01/06/21_tue_3_11.00-11.50_WT_PRSS</t>
+  </si>
+  <si>
+    <t>01/06/21_tue_4_12.00-12.50_OOSE_SVR/TR</t>
+  </si>
+  <si>
+    <t>01/06/21_tue_5,6_2.00-3.50_VA_MdRiaz</t>
+  </si>
+  <si>
+    <t>01/06/21_tue_7_4.00-4.50_SRP_NRD</t>
+  </si>
+  <si>
+    <t>02/06/21_wed_1_9.00-11.50_CC-II_PSR/Chandu</t>
+  </si>
+  <si>
+    <t>02/06/21_wed_4_12.00-12.50_CNS_BVDS/MKSV</t>
+  </si>
+  <si>
+    <t>02/06/21_wed_5,6,7_2.00-4.50_OOSE-LAB_SVR/TR</t>
+  </si>
+  <si>
+    <t>03/06/21_thu_1_9.00-9.50_OOSE_SVR/TR</t>
+  </si>
+  <si>
+    <t>03/06/21_thu_2_10.00-10.50_DWDBA_MVS/PNT</t>
+  </si>
+  <si>
+    <t>03/06/21_thu_3_11.00-11.50_CNS_BVDS/MKSV</t>
+  </si>
+  <si>
+    <t>03/06/21_thu_4_12.00-12.50_SRP_NRD</t>
+  </si>
+  <si>
+    <t>03/06/21_thu_5_2.00-2.50_WT_PRSS</t>
+  </si>
+  <si>
+    <t>03/06/21_thu_6_3.00-3.50_OR_CHGR/KSB</t>
+  </si>
+  <si>
+    <t>04/06/21_fri_1_9.00-9.50_DWDBA_MVS/PNT</t>
+  </si>
+  <si>
+    <t>04/06/21_fri_2_10.00-10.50_OR_CHGR/KSB</t>
+  </si>
+  <si>
+    <t>04/06/21_fri_3_11.00-11.50_OOSE_SVR/TR</t>
+  </si>
+  <si>
+    <t>04/06/21_fri_4_12.00-12.50_WT_PRSS</t>
+  </si>
+  <si>
+    <t>04/06/21_fri_5,6,7_2.00-4.50_WT LAB_PRSS</t>
+  </si>
+  <si>
+    <t>05/06/21_sat_1_9.00-9.50_CNS_BVDS/MKSV</t>
+  </si>
+  <si>
+    <t>05/06/21_sat_2_10.00-10.50_SRP_NRD</t>
+  </si>
+  <si>
+    <t>05/06/21_sat_3_11.00-11.50_DWDBA_MVS/PNT</t>
+  </si>
+  <si>
+    <t>05/06/21_sat_4_12.00-12.50_OR_CHGR/KSB</t>
+  </si>
+  <si>
+    <t>05/06/21_sat_5,6_2.00-3.50_IPR&amp;P_SR</t>
+  </si>
+  <si>
+    <t>First Class is not stoped</t>
   </si>
 </sst>
 </file>
@@ -810,7 +907,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -823,6 +920,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1140,7 +1240,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8039E4DD-5CE4-E44B-9CBA-DC1D8D4E8278}">
   <dimension ref="A1:F32"/>
   <sheetViews>
-    <sheetView topLeftCell="A11" zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
+    <sheetView topLeftCell="A21" zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
       <selection activeCell="A2" sqref="A2:F32"/>
     </sheetView>
   </sheetViews>
@@ -1168,7 +1268,7 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" s="1">
-        <v>44340</v>
+        <v>44347</v>
       </c>
       <c r="B2" t="s">
         <v>5</v>
@@ -1188,7 +1288,7 @@
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" s="1">
-        <v>44340</v>
+        <v>44347</v>
       </c>
       <c r="B3" t="s">
         <v>5</v>
@@ -1208,7 +1308,7 @@
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" s="1">
-        <v>44340</v>
+        <v>44347</v>
       </c>
       <c r="B4" t="s">
         <v>5</v>
@@ -1228,7 +1328,7 @@
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" s="1">
-        <v>44340</v>
+        <v>44347</v>
       </c>
       <c r="B5" t="s">
         <v>5</v>
@@ -1248,7 +1348,7 @@
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" s="1">
-        <v>44340</v>
+        <v>44347</v>
       </c>
       <c r="B6" t="s">
         <v>5</v>
@@ -1268,7 +1368,7 @@
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7" s="1">
-        <v>44340</v>
+        <v>44347</v>
       </c>
       <c r="B7" t="s">
         <v>5</v>
@@ -1288,7 +1388,7 @@
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8" s="1">
-        <v>44341</v>
+        <v>44348</v>
       </c>
       <c r="B8" t="s">
         <v>6</v>
@@ -1308,7 +1408,7 @@
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A9" s="1">
-        <v>44341</v>
+        <v>44348</v>
       </c>
       <c r="B9" t="s">
         <v>6</v>
@@ -1328,7 +1428,7 @@
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A10" s="1">
-        <v>44341</v>
+        <v>44348</v>
       </c>
       <c r="B10" t="s">
         <v>6</v>
@@ -1348,7 +1448,7 @@
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A11" s="1">
-        <v>44341</v>
+        <v>44348</v>
       </c>
       <c r="B11" t="s">
         <v>6</v>
@@ -1368,7 +1468,7 @@
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A12" s="1">
-        <v>44341</v>
+        <v>44348</v>
       </c>
       <c r="B12" t="s">
         <v>6</v>
@@ -1388,7 +1488,7 @@
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A13" s="1">
-        <v>44341</v>
+        <v>44348</v>
       </c>
       <c r="B13" t="s">
         <v>6</v>
@@ -1408,7 +1508,7 @@
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A14" s="4">
-        <v>44342</v>
+        <v>44349</v>
       </c>
       <c r="B14" t="s">
         <v>7</v>
@@ -1428,7 +1528,7 @@
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A15" s="4">
-        <v>44342</v>
+        <v>44349</v>
       </c>
       <c r="B15" t="s">
         <v>7</v>
@@ -1448,7 +1548,7 @@
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A16" s="4">
-        <v>44342</v>
+        <v>44349</v>
       </c>
       <c r="B16" t="s">
         <v>7</v>
@@ -1468,7 +1568,7 @@
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A17" s="4">
-        <v>44343</v>
+        <v>44350</v>
       </c>
       <c r="B17" t="s">
         <v>8</v>
@@ -1488,7 +1588,7 @@
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A18" s="4">
-        <v>44343</v>
+        <v>44350</v>
       </c>
       <c r="B18" t="s">
         <v>8</v>
@@ -1508,7 +1608,7 @@
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A19" s="4">
-        <v>44343</v>
+        <v>44350</v>
       </c>
       <c r="B19" t="s">
         <v>8</v>
@@ -1528,7 +1628,7 @@
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A20" s="4">
-        <v>44343</v>
+        <v>44350</v>
       </c>
       <c r="B20" t="s">
         <v>8</v>
@@ -1548,7 +1648,7 @@
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A21" s="4">
-        <v>44343</v>
+        <v>44350</v>
       </c>
       <c r="B21" t="s">
         <v>8</v>
@@ -1568,7 +1668,7 @@
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A22" s="4">
-        <v>44343</v>
+        <v>44350</v>
       </c>
       <c r="B22" t="s">
         <v>8</v>
@@ -1588,7 +1688,7 @@
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A23" s="1">
-        <v>44344</v>
+        <v>44351</v>
       </c>
       <c r="B23" t="s">
         <v>9</v>
@@ -1608,7 +1708,7 @@
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A24" s="1">
-        <v>44344</v>
+        <v>44351</v>
       </c>
       <c r="B24" t="s">
         <v>9</v>
@@ -1628,7 +1728,7 @@
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A25" s="1">
-        <v>44344</v>
+        <v>44351</v>
       </c>
       <c r="B25" t="s">
         <v>9</v>
@@ -1648,7 +1748,7 @@
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A26" s="1">
-        <v>44344</v>
+        <v>44351</v>
       </c>
       <c r="B26" t="s">
         <v>9</v>
@@ -1668,7 +1768,7 @@
     </row>
     <row r="27" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A27" s="1">
-        <v>44344</v>
+        <v>44351</v>
       </c>
       <c r="B27" t="s">
         <v>9</v>
@@ -1688,7 +1788,7 @@
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A28" s="1">
-        <v>44345</v>
+        <v>44352</v>
       </c>
       <c r="B28" t="s">
         <v>10</v>
@@ -1708,7 +1808,7 @@
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A29" s="1">
-        <v>44345</v>
+        <v>44352</v>
       </c>
       <c r="B29" t="s">
         <v>10</v>
@@ -1728,7 +1828,7 @@
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A30" s="1">
-        <v>44345</v>
+        <v>44352</v>
       </c>
       <c r="B30" t="s">
         <v>10</v>
@@ -1748,7 +1848,7 @@
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A31" s="1">
-        <v>44345</v>
+        <v>44352</v>
       </c>
       <c r="B31" t="s">
         <v>10</v>
@@ -1768,7 +1868,7 @@
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A32" s="1">
-        <v>44345</v>
+        <v>44352</v>
       </c>
       <c r="B32" t="s">
         <v>10</v>
@@ -3113,8 +3213,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{09DB4D99-4C78-A244-B49A-974962952A2A}">
   <dimension ref="B7:F37"/>
   <sheetViews>
-    <sheetView topLeftCell="A28" zoomScale="150" workbookViewId="0">
-      <selection activeCell="C23" sqref="C23:C50"/>
+    <sheetView zoomScale="150" workbookViewId="0">
+      <selection activeCell="E48" sqref="E48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3489,11 +3589,381 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B40387AC-8F51-0045-B833-B21ECBA86850}">
+  <dimension ref="B5:E35"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A18" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="B35" sqref="B35"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="3" max="3" width="44.83203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="20.83203125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="5" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B5">
+        <v>1</v>
+      </c>
+      <c r="C5" t="s">
+        <v>240</v>
+      </c>
+      <c r="D5" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="6" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B6">
+        <v>2</v>
+      </c>
+      <c r="C6" t="s">
+        <v>241</v>
+      </c>
+      <c r="D6" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="7" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B7">
+        <v>3</v>
+      </c>
+      <c r="C7" t="s">
+        <v>242</v>
+      </c>
+      <c r="D7" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="8" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B8">
+        <v>4</v>
+      </c>
+      <c r="C8" t="s">
+        <v>243</v>
+      </c>
+      <c r="D8" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="9" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B9">
+        <v>5</v>
+      </c>
+      <c r="C9" t="s">
+        <v>244</v>
+      </c>
+      <c r="D9" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="10" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B10">
+        <v>6</v>
+      </c>
+      <c r="C10" t="s">
+        <v>245</v>
+      </c>
+      <c r="D10" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="11" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B11">
+        <v>7</v>
+      </c>
+      <c r="C11" t="s">
+        <v>246</v>
+      </c>
+      <c r="D11" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="12" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B12">
+        <v>8</v>
+      </c>
+      <c r="C12" t="s">
+        <v>247</v>
+      </c>
+      <c r="D12" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="13" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B13">
+        <v>9</v>
+      </c>
+      <c r="C13" t="s">
+        <v>248</v>
+      </c>
+      <c r="D13" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="14" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B14">
+        <v>10</v>
+      </c>
+      <c r="C14" t="s">
+        <v>249</v>
+      </c>
+      <c r="D14" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="15" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B15">
+        <v>11</v>
+      </c>
+      <c r="C15" t="s">
+        <v>250</v>
+      </c>
+      <c r="D15" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="16" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B16">
+        <v>12</v>
+      </c>
+      <c r="C16" t="s">
+        <v>251</v>
+      </c>
+      <c r="D16" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="17" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B17">
+        <v>13</v>
+      </c>
+      <c r="C17" t="s">
+        <v>252</v>
+      </c>
+      <c r="D17" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="18" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B18">
+        <v>14</v>
+      </c>
+      <c r="C18" t="s">
+        <v>253</v>
+      </c>
+      <c r="D18" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="19" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B19">
+        <v>15</v>
+      </c>
+      <c r="C19" t="s">
+        <v>254</v>
+      </c>
+      <c r="D19" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="20" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B20">
+        <v>16</v>
+      </c>
+      <c r="C20" t="s">
+        <v>255</v>
+      </c>
+      <c r="D20" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="21" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B21">
+        <v>17</v>
+      </c>
+      <c r="C21" t="s">
+        <v>256</v>
+      </c>
+      <c r="D21" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="22" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B22">
+        <v>18</v>
+      </c>
+      <c r="C22" t="s">
+        <v>257</v>
+      </c>
+      <c r="D22" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="23" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B23">
+        <v>19</v>
+      </c>
+      <c r="C23" t="s">
+        <v>258</v>
+      </c>
+      <c r="D23" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="24" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B24">
+        <v>20</v>
+      </c>
+      <c r="C24" t="s">
+        <v>259</v>
+      </c>
+      <c r="D24" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="25" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B25">
+        <v>21</v>
+      </c>
+      <c r="C25" t="s">
+        <v>260</v>
+      </c>
+      <c r="D25" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="26" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B26">
+        <v>22</v>
+      </c>
+      <c r="C26" t="s">
+        <v>261</v>
+      </c>
+      <c r="D26" t="s">
+        <v>52</v>
+      </c>
+      <c r="E26" s="7" t="s">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="27" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B27">
+        <v>23</v>
+      </c>
+      <c r="C27" t="s">
+        <v>262</v>
+      </c>
+      <c r="D27" t="s">
+        <v>52</v>
+      </c>
+      <c r="E27" s="7"/>
+    </row>
+    <row r="28" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B28">
+        <v>24</v>
+      </c>
+      <c r="C28" t="s">
+        <v>263</v>
+      </c>
+      <c r="D28" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="29" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B29">
+        <v>25</v>
+      </c>
+      <c r="C29" t="s">
+        <v>264</v>
+      </c>
+      <c r="D29" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="30" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B30">
+        <v>26</v>
+      </c>
+      <c r="C30" t="s">
+        <v>265</v>
+      </c>
+      <c r="D30" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="31" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B31">
+        <v>27</v>
+      </c>
+      <c r="C31" t="s">
+        <v>266</v>
+      </c>
+      <c r="D31" t="s">
+        <v>52</v>
+      </c>
+      <c r="E31" s="7" t="s">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="32" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B32">
+        <v>28</v>
+      </c>
+      <c r="C32" t="s">
+        <v>267</v>
+      </c>
+      <c r="D32" t="s">
+        <v>52</v>
+      </c>
+      <c r="E32" s="7"/>
+    </row>
+    <row r="33" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B33">
+        <v>29</v>
+      </c>
+      <c r="C33" t="s">
+        <v>268</v>
+      </c>
+      <c r="D33" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="34" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B34">
+        <v>30</v>
+      </c>
+      <c r="C34" t="s">
+        <v>269</v>
+      </c>
+      <c r="D34" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="35" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B35">
+        <v>31</v>
+      </c>
+      <c r="C35" t="s">
+        <v>270</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="E26:E27"/>
+    <mergeCell ref="E31:E32"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D2D23755-A581-8342-8C84-D7823222C627}">
   <dimension ref="B7:E38"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A18" zoomScale="174" zoomScaleNormal="174" workbookViewId="0">
-      <selection activeCell="D38" sqref="D38"/>
+    <sheetView zoomScale="174" zoomScaleNormal="174" workbookViewId="0">
+      <selection activeCell="G29" sqref="G29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3872,6 +4342,9 @@
       <c r="D38" t="s">
         <v>237</v>
       </c>
+      <c r="E38" t="s">
+        <v>52</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>